<commit_message>
List Of Engineering College In Greater Noida
</commit_message>
<xml_diff>
--- a/Documents/List Of 10 Engineering College In Greater Noida/List Of Engineering College In Greater Noida.xlsx
+++ b/Documents/List Of 10 Engineering College In Greater Noida/List Of Engineering College In Greater Noida.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Name Of College</t>
   </si>
@@ -40,30 +40,6 @@
     <t>Support@galgotiacollege.edu</t>
   </si>
   <si>
-    <r>
-      <t>www.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>galgotiacollege</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.edu</t>
-    </r>
-  </si>
-  <si>
     <t>Skyline Institute Of Engineering &amp; Technology</t>
   </si>
   <si>
@@ -73,70 +49,122 @@
     <t xml:space="preserve">         0120 232 0206</t>
   </si>
   <si>
-    <r>
-      <t>skylineinstitute</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.com</t>
-    </r>
-  </si>
-  <si>
     <t> info@skylineinstitute.com</t>
   </si>
   <si>
-    <r>
-      <t>www.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>niet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF006621"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.co.in</t>
-    </r>
-  </si>
-  <si>
     <t>19, IILM Road, Knowledge Park II, Institutional Area, Greater Noida, Uttar Pradesh 201310</t>
   </si>
   <si>
     <t xml:space="preserve">      0120 232 0132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N.I.E.T Engineering College </t>
+  </si>
+  <si>
+    <t>G.N.I.E.T Engineering College</t>
+  </si>
+  <si>
+    <t>Plot No. 7, Knowledge Park - II, Greater Noida, Uttar Pradesh 201308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       092506 44422</t>
+  </si>
+  <si>
+    <t>gniotgroup.edu.in</t>
+  </si>
+  <si>
+    <t>http://www.gnit.net</t>
+  </si>
+  <si>
+    <t>49, Knowledge Park-III, Greater Noida, Uttar Pradesh 201306</t>
+  </si>
+  <si>
+    <t>info@accurate.in</t>
+  </si>
+  <si>
+    <t>http://www.accurate.in</t>
+  </si>
+  <si>
+    <t>0120-2328234/35</t>
+  </si>
+  <si>
+    <t>Accurate Institute of Management &amp; Technology</t>
+  </si>
+  <si>
+    <t>I.T.S Engineering College Greater Noida</t>
+  </si>
+  <si>
+    <t>46, Knowledge Park-III, Greater Noida-201308</t>
+  </si>
+  <si>
+    <t>director.office.ec@its.edu.in</t>
+  </si>
+  <si>
+    <t>http://www.itsecgn.edu.in</t>
+  </si>
+  <si>
+    <t>http://www.niet.co.in</t>
+  </si>
+  <si>
+    <t>http://www.galgotiacollege.edu</t>
+  </si>
+  <si>
+    <t>http://skylineinstitute.com</t>
+  </si>
+  <si>
+    <t>Priyadarshini College of computer science</t>
+  </si>
+  <si>
+    <t>info@pccscampus.com</t>
+  </si>
+  <si>
+    <t>http://www.pccscampus.com</t>
+  </si>
+  <si>
+    <t>Plot no-6A &amp;7 instutional Area Knowledge Park 1 Greater Noida 201306</t>
+  </si>
+  <si>
+    <t>I.E.C Group Of Institution</t>
+  </si>
+  <si>
+    <t>Plot No. 4, Institutional Area, Surajpur Kasna Road Greater Noida 201306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           120-2326665</t>
+  </si>
+  <si>
+    <t>enquiry@ieccollege.com</t>
+  </si>
+  <si>
+    <t>www.ieccollege.com </t>
+  </si>
+  <si>
+    <t>Plot No. 2, Knowledge Park III,Distt. G.B.Nagar, Greater Noida, Uttar Pradesh 201306</t>
+  </si>
+  <si>
+    <t>G.L Bajaj Institute Of Engineering &amp; Technology</t>
+  </si>
+  <si>
+    <t>info@glbitm.org</t>
+  </si>
+  <si>
+    <t>http://www.glbitm.org</t>
+  </si>
+  <si>
+    <t>admission.niet.co.in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF333333"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -152,13 +180,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF006621"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
@@ -167,6 +188,33 @@
     <font>
       <sz val="9"/>
       <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF43433C"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF535353"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -196,20 +244,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -517,19 +567,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="43.7109375" customWidth="1"/>
-    <col min="2" max="2" width="70.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.42578125" customWidth="1"/>
+    <col min="2" max="2" width="72.28515625" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1">
@@ -553,58 +603,173 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1204370000</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5" s="2"/>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>1202331000</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>1202322750</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>1202323818</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="mailto:Support@galgotiacollege.edu"/>
     <hyperlink ref="D3" r:id="rId2" display="mailto:info@skylineinstitute.com"/>
+    <hyperlink ref="E5" r:id="rId3"/>
+    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E7" r:id="rId5"/>
+    <hyperlink ref="E4" r:id="rId6"/>
+    <hyperlink ref="E2" r:id="rId7"/>
+    <hyperlink ref="E3" r:id="rId8"/>
+    <hyperlink ref="D8" r:id="rId9"/>
+    <hyperlink ref="E8" r:id="rId10"/>
+    <hyperlink ref="D9" r:id="rId11" display="mailto:enquiry@ieccollege.com"/>
+    <hyperlink ref="E9" r:id="rId12" display="http://www.ieccollege.com/"/>
+    <hyperlink ref="E10" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>